<commit_message>
hadoop data transfer related information
git-svn-id: file://localhost/tmp/svn2git/svn@6647 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/mrworkshop12/data/Final_Data.xlsx
+++ b/papers/mrworkshop12/data/Final_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28780" yWindow="-7940" windowWidth="25040" windowHeight="14240" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="12620" yWindow="-20" windowWidth="12860" windowHeight="14100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="wc hadoop-pmr" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="197">
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.48% of intermediate transfer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediate data in case of PMR is 18468MB for 20GB whichis 92%</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediate data in case of PMR is 36454.269MB  for 40GB whichis 91.4%</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>98% intermediate data generated.</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -277,518 +301,514 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>31.2% of intermediate transfer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actual data transfer time is 610 seconcds.. But local data transfer is considered as negligible..</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14 mintues remote</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 minutes local</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> in 14 minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remote Data in MB transferred to India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machines</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermdiate data generated in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer local data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;1sec</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average reduce data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Total data exchanged is </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. if its reduce intensive , then it takes more time.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. it is forced to move the data to location where data transfer is high..</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. With efficient file transfer protocols, pilot-DMR proves to be better.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local PMR on 6240MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transfer 3120MB using SCP</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 LOCAL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 to B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 to LOCAL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 to A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>negligible file transfer time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 has to be distributed to 8 reduces on B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 has to be distiuted to 8 reduces on A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distribution of data to each Reduce</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;1minute</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remote Data in MB transferred</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local Data in MB transferred</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>exchanged.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of MR </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR for  jon's DMR and distibuted-PMR.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>16GB wordcount , local mr, 8 workers, 128MB chunk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transferred between map and reduce phase</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machines used India, hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffletime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce phase</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediatedata</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduces</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-5r</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>rreduce-6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of concurent transfers</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>effective data transfer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>total intermediate data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>30GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>60GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>60GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 5932 MB from hotel-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (5932*3) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>120GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>30GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 8946 MB from hotel-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (8946*3) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distributed-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>120GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of concurrent pilot transfers are 8*(2-1)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB divided into 10GB on india, 10GB hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hadoop MR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 8946 MB from India-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (8946*2) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB(replicated)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqeuences</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB(replicated)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>dmr stderr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>pmrstderr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on 9360 MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on 6240 MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 3120MB from hotel-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffletime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce phase</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>effective data transfer involved in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total intermediate data produced in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Input data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>12.48% of intermediate transfer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>31.2% of intermediate transfer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Actual data transfer time is 610 seconcds.. But local data transfer is considered as negligible..</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>18 minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>14 mintues remote</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 minutes local</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>14minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> in 14 minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remote Data in MB transferred to India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machines</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intermdiate data generated in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer local data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;1sec</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average reduce data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Total data exchanged is </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. if its reduce intensive , then it takes more time.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. it is forced to move the data to location where data transfer is high..</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. With efficient file transfer protocols, pilot-DMR proves to be better.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local PMR on 6240MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Transfer 3120MB using SCP</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>9GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 LOCAL</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 to B</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 to LOCAL</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 to A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>negligible file transfer time</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 has to be distributed to 8 reduces on B</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 has to be distiuted to 8 reduces on A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Distribution of data to each Reduce</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;1minute</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remote Data in MB transferred</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local Data in MB transferred</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>exchanged.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of MR </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR for  jon's DMR and distibuted-PMR.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>16GB wordcount , local mr, 8 workers, 128MB chunk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transferred between map and reduce phase</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machines used India, hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chunk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffletime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce phase</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intermediatedata</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduces</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-4</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-5r</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>rreduce-6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-7</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of concurent transfers</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>effective data transfer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>total intermediate data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>30GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>60GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>60GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 5932 MB from hotel-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (5932*3) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>average</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>120GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>30GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 8946 MB from hotel-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (8946*3) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Distributed-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>120GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of concurrent pilot transfers are 8*(2-1)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB divided into 10GB on india, 10GB hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hadoop MR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>average</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>40GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>80GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 8946 MB from India-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (8946*2) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>80GB(replicated)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqeuences</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>80GB(replicated)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>40GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>80GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>dmr stderr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>pmrstderr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on 9360 MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on 6240 MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 3120MB from hotel-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chunk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffletime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce phase</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>effective data transfer involved in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total intermediate data produced in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-0</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1185,11 +1205,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="464698408"/>
-        <c:axId val="464689272"/>
+        <c:axId val="493649544"/>
+        <c:axId val="493655336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="464698408"/>
+        <c:axId val="493649544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1210,18 +1230,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="464689272"/>
+        <c:crossAx val="493655336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="464689272"/>
+        <c:axId val="493655336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,11 +1261,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="464698408"/>
+        <c:crossAx val="493649544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1608,24 +1626,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="542508216"/>
-        <c:axId val="542505064"/>
+        <c:axId val="493688808"/>
+        <c:axId val="493691944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="542508216"/>
+        <c:axId val="493688808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542505064"/>
+        <c:crossAx val="493691944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="542505064"/>
+        <c:axId val="493691944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1633,14 +1651,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542508216"/>
+        <c:crossAx val="493688808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1664,8 +1681,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127972690122595"/>
-          <c:y val="0.0509259259259259"/>
+          <c:x val="0.0899980065782916"/>
+          <c:y val="0.123041338582677"/>
           <c:w val="0.793585567626831"/>
           <c:h val="0.7261402741324"/>
         </c:manualLayout>
@@ -1877,11 +1894,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="542437128"/>
-        <c:axId val="542427368"/>
+        <c:axId val="493754808"/>
+        <c:axId val="493764376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="542437128"/>
+        <c:axId val="493754808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,14 +1922,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542427368"/>
+        <c:crossAx val="493764376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="542427368"/>
+        <c:axId val="493764376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1937,7 +1954,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542437128"/>
+        <c:crossAx val="493754808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2147,31 +2164,31 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="542338328"/>
-        <c:axId val="542335256"/>
+        <c:axId val="493853320"/>
+        <c:axId val="493856376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="542338328"/>
+        <c:axId val="493853320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542335256"/>
+        <c:crossAx val="493856376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="542335256"/>
+        <c:axId val="493856376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542338328"/>
+        <c:crossAx val="493853320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2260,15 +2277,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>647700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>647700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2285,6 +2302,56 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:ma="http://schemas.microsoft.com/office/mac/drawingml/2008/main" Requires="ma">
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+        </mc:Choice>
+        <mc:Fallback>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+        </mc:Fallback>
+      </mc:AlternateContent>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7073900" y="23114000"/>
+          <a:ext cx="5829300" cy="5651500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2655,7 +2722,7 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="B2" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -2665,45 +2732,45 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="26">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2832,33 +2899,33 @@
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1">
       <c r="A22" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" ht="78">
       <c r="A24" s="4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2998,13 +3065,13 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="2" customFormat="1"/>
     <row r="43" spans="1:14">
       <c r="J43" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -3042,24 +3109,24 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B46">
         <v>164.37300000000002</v>
@@ -3078,7 +3145,7 @@
         <v>2208.0443333333333</v>
       </c>
       <c r="H46" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I46" s="5">
         <v>684.23799999999994</v>
@@ -3098,7 +3165,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B47" s="1">
         <v>138.96699999999998</v>
@@ -3117,7 +3184,7 @@
         <v>2123.8213333333333</v>
       </c>
       <c r="H47" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I47" s="5">
         <v>473.4563333333333</v>
@@ -3137,7 +3204,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="H48" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I48">
         <v>33.993099001840605</v>
@@ -3157,7 +3224,7 @@
     </row>
     <row r="49" spans="8:13">
       <c r="H49" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I49">
         <v>127.57381609687643</v>
@@ -3219,6 +3286,7 @@
       <c r="G81" s="5"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -3234,8 +3302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3246,12 +3314,12 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>32</v>
@@ -3259,23 +3327,23 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -3284,7 +3352,7 @@
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -3296,26 +3364,26 @@
     </row>
     <row r="8" spans="1:12" s="10" customFormat="1" ht="65">
       <c r="A8" s="19" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G8" s="19"/>
       <c r="I8" s="19" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3340,7 +3408,7 @@
         <v>3120</v>
       </c>
       <c r="K9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3362,14 +3430,14 @@
         <v>2681.3405951185346</v>
       </c>
       <c r="F10" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G10">
         <f>AVERAGE(E9:E11)</f>
         <v>2652.2825510560347</v>
       </c>
       <c r="H10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="I10">
         <v>19029605</v>
@@ -3394,24 +3462,24 @@
         <v>2570.3256126185343</v>
       </c>
       <c r="F11" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G11">
         <f>1.96*(STDEV(E9:E11)/SQRT(3))</f>
         <v>81.442668757892889</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="K12" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="E14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H14">
         <f>(F9-F17)/F17*100</f>
@@ -3426,25 +3494,25 @@
     </row>
     <row r="16" spans="1:12" ht="65">
       <c r="A16" s="22" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -3473,7 +3541,7 @@
         <v>19100</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -3495,7 +3563,7 @@
         <v>2256.0450000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G18">
         <f>AVERAGE(E17:E19)</f>
@@ -3521,7 +3589,7 @@
         <v>2245.4900000000002</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G19">
         <f>1.96*(STDEV(E17:E19)/SQRT(3))</f>
@@ -3530,21 +3598,21 @@
     </row>
     <row r="21" spans="1:14">
       <c r="J21" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="K21" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="L21" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="M21" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="I22" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="J22">
         <v>2652.2825510560347</v>
@@ -3565,7 +3633,7 @@
     </row>
     <row r="23" spans="1:14">
       <c r="I23" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="J23">
         <v>4528.8221494252866</v>
@@ -3586,7 +3654,7 @@
     </row>
     <row r="24" spans="1:14">
       <c r="I24" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="J24">
         <v>8375.575505747127</v>
@@ -3607,7 +3675,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="I25" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="J25">
         <v>7606.7479195402293</v>
@@ -3632,7 +3700,7 @@
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -3644,22 +3712,22 @@
     </row>
     <row r="28" spans="1:14" ht="65">
       <c r="A28" s="19" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -3705,7 +3773,7 @@
         <v>4832.7978160919538</v>
       </c>
       <c r="F30" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G30">
         <f>AVERAGE(E29:E31)</f>
@@ -3732,7 +3800,7 @@
         <v>4712.2308160919538</v>
       </c>
       <c r="F31" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G31">
         <f>1.96*(STDEV(E29:E31)/SQRT(3))</f>
@@ -3745,37 +3813,55 @@
         <f>(F29-F41)/F41*100</f>
         <v>138.52030558906313</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="M32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="M33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="M34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="H37">
         <f>(G30-G42)/G42*100</f>
         <v>12.933088628712127</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="65">
+    <row r="40" spans="1:13" ht="65">
       <c r="A40" s="16" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41">
         <f>506.48/2</f>
         <v>253.24</v>
@@ -3802,8 +3888,19 @@
 18456</f>
         <v>36912</v>
       </c>
-    </row>
-    <row r="42" spans="1:9">
+      <c r="H41">
+        <v>18468</v>
+      </c>
+      <c r="I41">
+        <f>2.487/20</f>
+        <v>0.12435</v>
+      </c>
+      <c r="J41">
+        <f>2.12/18.46</f>
+        <v>0.11484290357529794</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42">
         <v>260.43</v>
       </c>
@@ -3822,17 +3919,17 @@
         <v>4273.09</v>
       </c>
       <c r="F42" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G42">
         <f>AVERAGE(E41:E43)</f>
         <v>4239.8133333333335</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43">
         <v>264.32</v>
       </c>
@@ -3850,7 +3947,7 @@
         <v>4174.5200000000004</v>
       </c>
       <c r="F43" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G43">
         <f>1.96*(STDEV(E41:E43)/SQRT(3))</f>
@@ -3861,25 +3958,25 @@
         <v>38059210</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:13">
       <c r="H45" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="C46" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F46" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:12" s="21" customFormat="1">
       <c r="E52" s="21" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3887,22 +3984,22 @@
     </row>
     <row r="54" spans="1:12" ht="65">
       <c r="A54" s="19" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3947,7 +4044,7 @@
         <v>8410.8611724137936</v>
       </c>
       <c r="F56" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G56">
         <f>AVERAGE(E55:E57)</f>
@@ -3973,7 +4070,7 @@
         <v>8354.4101724137927</v>
       </c>
       <c r="F57" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G57">
         <f>1.96*(STDEV(E55:E57)/SQRT(3))</f>
@@ -3982,25 +4079,25 @@
     </row>
     <row r="59" spans="1:12" ht="65">
       <c r="A59" s="16" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -4025,6 +4122,10 @@
       <c r="F60" s="17">
         <v>4425</v>
       </c>
+      <c r="G60">
+        <f>4.425/40</f>
+        <v>0.110625</v>
+      </c>
       <c r="I60">
         <f>38059210*2</f>
         <v>76118420</v>
@@ -4051,7 +4152,7 @@
         <v>7794.87</v>
       </c>
       <c r="F61" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G61">
         <f>AVERAGE(E60:E62)</f>
@@ -4078,7 +4179,7 @@
         <v>7905.7</v>
       </c>
       <c r="F62" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G62">
         <f>1.96*(STDEV(E60:E62)/SQRT(3))</f>
@@ -4091,29 +4192,34 @@
         <v>102.16949152542374</v>
       </c>
     </row>
+    <row r="65" spans="1:10">
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="66" spans="1:10" s="21" customFormat="1">
       <c r="E66" s="21" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="65">
       <c r="A70" s="19" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -4162,7 +4268,7 @@
         <v>7622.033586206896</v>
       </c>
       <c r="F72" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G72">
         <f>AVERAGE(E71:E73)</f>
@@ -4195,7 +4301,7 @@
         <v>7585.5825862068959</v>
       </c>
       <c r="F73" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G73">
         <f>1.96*(STDEV(E71:E73)/SQRT(3))</f>
@@ -4209,6 +4315,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4228,130 +4335,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="2:8">
       <c r="C1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:8">
       <c r="C3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="G7" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="C8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" t="s">
         <v>102</v>
       </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" t="s">
-        <v>98</v>
-      </c>
       <c r="G10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="2:8">
       <c r="G11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="39">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="2" customFormat="1">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C21">
         <v>9862</v>
@@ -4368,7 +4475,7 @@
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -4417,10 +4524,10 @@
         <v>9267</v>
       </c>
       <c r="H26" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I26" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -4436,7 +4543,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="B28" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C28">
         <v>9838</v>
@@ -4475,58 +4582,58 @@
     </row>
     <row r="32" spans="1:12">
       <c r="D32" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="C34" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="52">
       <c r="A40" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K40" s="16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C41">
         <v>9862</v>
@@ -4540,7 +4647,7 @@
         <v>4604</v>
       </c>
       <c r="F41" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G41">
         <v>7</v>
@@ -4554,7 +4661,7 @@
         <v>9267</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K41" s="17">
         <f>MAX('10GB'!E21:E24,'10GB'!E27:E30)</f>
@@ -4563,10 +4670,10 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>9838</v>
@@ -4580,7 +4687,7 @@
         <v>4663</v>
       </c>
       <c r="F42" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G42">
         <v>7</v>
@@ -4593,7 +4700,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="J43" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K43" s="17">
         <f>3120</f>
@@ -4601,6 +4708,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4616,46 +4724,46 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:12" ht="65">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2">
         <v>18468</v>
@@ -4669,17 +4777,17 @@
         <v>9184</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H2">
         <f>SUM(D2:D3)</f>
         <v>18456</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K2" s="17">
         <f>MAX(E11:E14,E17:E20)</f>
@@ -4692,10 +4800,10 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>18468</v>
@@ -4709,10 +4817,10 @@
         <v>9296</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H3">
         <f>SUM(D2:D3)</f>
@@ -4722,7 +4830,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="J4" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4" s="17">
         <f>2980+2985</f>
@@ -4731,27 +4839,27 @@
     </row>
     <row r="10" spans="1:12" ht="52">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11">
         <v>18468</v>
@@ -4799,18 +4907,18 @@
         <v>4552</v>
       </c>
       <c r="I14" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="D16" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -4826,7 +4934,7 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C18">
         <v>18468</v>
@@ -4864,8 +4972,10 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4876,49 +4986,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:11" ht="65">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2">
         <v>36454.269</v>
@@ -4932,17 +5042,17 @@
         <v>17233</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <f>SUM(D2:D3)</f>
         <v>34978</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K2" s="17">
         <f>MAX(E11:E14,E17:E20)</f>
@@ -4951,10 +5061,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>36454.269</v>
@@ -4968,10 +5078,10 @@
         <v>17123</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <f>SUM(D2:D3)</f>
@@ -4981,7 +5091,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="J4" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4" s="17">
         <f>5952</f>
@@ -4990,27 +5100,27 @@
     </row>
     <row r="10" spans="1:11" ht="52">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11">
         <v>36454.269</v>
@@ -5044,7 +5154,7 @@
         <v>12.138496042809143</v>
       </c>
       <c r="I12" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -5079,13 +5189,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="D16" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -5105,10 +5215,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C18">
         <v>36454.269</v>
@@ -5157,7 +5267,14 @@
         <v>0.22942386831275721</v>
       </c>
     </row>
+    <row r="25" spans="1:8">
+      <c r="D25">
+        <f>36.54/40</f>
+        <v>0.91349999999999998</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5173,8 +5290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5188,7 +5305,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -5200,25 +5317,25 @@
     </row>
     <row r="2" spans="1:16" ht="65">
       <c r="A2" s="19" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H2" s="19"/>
       <c r="O2">
@@ -5282,7 +5399,7 @@
         <v>3014.5888529310346</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H4">
         <f>AVERAGE(F3:F5)</f>
@@ -5318,7 +5435,7 @@
         <v>2882.3651829310347</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H5">
         <f>1.96*(STDEV(F3:F5)/SQRT(3))</f>
@@ -5354,25 +5471,25 @@
     </row>
     <row r="11" spans="1:16" ht="65">
       <c r="A11" s="22" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -5401,13 +5518,13 @@
         <v>28396</v>
       </c>
       <c r="L12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="M12" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N12" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -5429,14 +5546,14 @@
         <v>2363.4366666666665</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G13">
         <f>AVERAGE(E12:E14)</f>
         <v>2416.8599999999997</v>
       </c>
       <c r="K13" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="L13">
         <v>2984.3501395977014</v>
@@ -5467,14 +5584,14 @@
         <v>2433.6466666666665</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G14">
         <f>1.96*(STDEV(E12:E14)/SQRT(3))</f>
         <v>53.54597837390223</v>
       </c>
       <c r="K14" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="L14">
         <v>2416.8599999999997</v>
@@ -5485,7 +5602,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="K17" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="L17">
         <v>102.66744486459044</v>
@@ -5499,7 +5616,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="K18" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="L18">
         <v>53.54597837390223</v>
@@ -5514,7 +5631,7 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
@@ -5526,25 +5643,25 @@
     </row>
     <row r="22" spans="1:14" ht="65">
       <c r="A22" s="19" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -5596,7 +5713,7 @@
         <v>5459.8978160919542</v>
       </c>
       <c r="G24" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H24">
         <f>AVERAGE(F23:F25)</f>
@@ -5626,7 +5743,7 @@
         <v>5623.6078160919533</v>
       </c>
       <c r="G25" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H25">
         <f>1.96*(STDEV(F23:F25)/SQRT(3))</f>
@@ -5642,25 +5759,25 @@
     </row>
     <row r="29" spans="1:14" ht="65">
       <c r="A29" s="22" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -5708,7 +5825,7 @@
         <v>4258.99</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="G31">
         <f>AVERAGE(E30:E32)</f>
@@ -5733,7 +5850,7 @@
         <v>4414.45</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G32">
         <f>1.96*(STDEV(E30:E32)/SQRT(3))</f>
@@ -5755,7 +5872,7 @@
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
       <c r="E36" s="21" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
@@ -5767,25 +5884,25 @@
     </row>
     <row r="37" spans="1:12" ht="65">
       <c r="A37" s="19" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -5836,7 +5953,7 @@
         <v>9408.8711724137938</v>
       </c>
       <c r="G39" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H39">
         <f>AVERAGE(F38:F40)</f>
@@ -5865,7 +5982,7 @@
         <v>9256.9201724137929</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H40">
         <f>1.96*(STDEV(F38:F40)/SQRT(3))</f>
@@ -5880,25 +5997,25 @@
     </row>
     <row r="44" spans="1:12" ht="65">
       <c r="A44" s="22" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -5919,6 +6036,7 @@
       <c r="F47" s="20"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -5934,8 +6052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A4:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5953,45 +6071,45 @@
     </row>
     <row r="7" spans="1:12" ht="39">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C8">
         <v>9862</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <f>SUM(F8:H8)</f>
@@ -6010,12 +6128,12 @@
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E9">
         <f>SUM(F9:H9)</f>
@@ -6036,7 +6154,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="D10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E10">
         <f>SUM(F10:H10)</f>
@@ -6057,18 +6175,18 @@
     </row>
     <row r="11" spans="1:12">
       <c r="L11" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>9267</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E12">
         <v>3463</v>
@@ -6092,7 +6210,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="D13" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E13">
         <v>3568</v>
@@ -6112,7 +6230,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="D14" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E14">
         <v>3566</v>
@@ -6132,7 +6250,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="K15" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -6143,13 +6261,13 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C17">
         <v>9267</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E17">
         <v>3531</v>
@@ -6169,7 +6287,7 @@
     </row>
     <row r="18" spans="2:10">
       <c r="D18" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E18">
         <v>3904</v>
@@ -6188,9 +6306,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6211,45 +6329,45 @@
   <sheetData>
     <row r="7" spans="1:12" ht="39">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C8">
         <v>18468</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <f>SUM(F8:H8)</f>
@@ -6268,12 +6386,12 @@
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E9">
         <f>SUM(F9:H9)</f>
@@ -6294,7 +6412,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="D10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E10">
         <f>SUM(F10:H10)</f>
@@ -6315,18 +6433,18 @@
     </row>
     <row r="11" spans="1:12">
       <c r="L11" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C12">
         <v>18468</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E12">
         <f>SUM(F12:H12)</f>
@@ -6351,7 +6469,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="D13" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E13">
         <f>SUM(F13:H13)</f>
@@ -6372,7 +6490,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="D14" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E14">
         <f>SUM(F14:H14)</f>
@@ -6393,7 +6511,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="K15" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -6404,13 +6522,13 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C17">
         <v>18468</v>
       </c>
       <c r="D17" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E17">
         <f>SUM(F17:H17)</f>
@@ -6431,7 +6549,7 @@
     </row>
     <row r="18" spans="2:10">
       <c r="D18" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E18">
         <f>SUM(F18:H18)</f>
@@ -6452,10 +6570,11 @@
     </row>
     <row r="25" spans="2:10">
       <c r="H25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -6474,6 +6593,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
removed hyphen in figures
git-svn-id: file://localhost/tmp/svn2git/svn@6767 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/mrworkshop12/data/Final_Data.xlsx
+++ b/papers/mrworkshop12/data/Final_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29060" yWindow="-7360" windowWidth="26740" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="35840" yWindow="520" windowWidth="21600" windowHeight="14120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="wc hadoop-pmr" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,667 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="228">
+  <si>
+    <t>Combine LMR on (8946*2) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB(replicated)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqeuences</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> in 14 minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remote Data in MB transferred to India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machines</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermdiate data generated in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer local data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;1sec</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average reduce data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Total data exchanged is </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. if its reduce intensive , then it takes more time.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. it is forced to move the data to location where data transfer is high..</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. With efficient file transfer protocols, pilot-DMR proves to be better.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local PMR on 6240MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transfer 3120MB using SCP</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>9GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 LOCAL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>parmiko</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>6GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>10GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of concurent transfers</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>effective data transfer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 5952 MB from India-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (5952*2) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffletime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce phase</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (5932*2) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 5932 MB from India-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>29minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> in 29 minutes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>29mins</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local Data in MB transferred within India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>time taken to distribute data to remote machines</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14mins</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;1min</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote Data in MB transferred to </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> effective data transfer in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>remote data distribution= 7mins</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR on India</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR on Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 3120MB from India-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>total intermediate data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>30GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>60GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>60GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 5932 MB from hotel-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (5932*3) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>120GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>30GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 8946 MB from hotel-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combine LMR on (8946*3) MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distributed-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>120GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of concurrent pilot transfers are 8*(2-1)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB divided into 10GB on india, 10GB hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hadoop MR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>20GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>40GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>80GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to transfer 8946 MB from India-&gt;hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>14 mintues remote</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 minutes local</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR-setup</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR-Map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR-Shuffle</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR-Reduce</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediate data in case of PMR is 18468MB for 20GB whichis 92%</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR on Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hadoop MR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for total</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr ofr pmr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for hmr</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hadoop</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>India,8workers,1woker/node, 128MB chunk, 8 reduces,varying input data size(GB)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>default replication factor - 2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>scp</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>paramiko</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>File in GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCP</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paramiko</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>t-scp% of t-paramiko</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data size in GB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>effective data transfer in GB in HMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>effective data transfer in GB in PMR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>%improvement of PMR(paramiko) over HMR(SCP)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>%improvement of PMR(SCP) over HMR(SCP)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 to B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 to LOCAL</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.5 to A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>negligible file transfer time</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>effective data transfer involved in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total intermediate data produced in MB</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>of weissmann paper..</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>related work</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>running bulk of applications on setup of machines.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>16GB wordcount , local mr, 8 workers, 128MB chunk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transferred between map and reduce phase</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machines used India, hotel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffletime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce phase</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediatedata</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduces</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-5r</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>rreduce-6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce-7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>tts(scp)</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -273,650 +933,6 @@
   </si>
   <si>
     <t>18 minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>14 mintues remote</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 minutes local</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR-setup</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR-Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR-Shuffle</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR-Reduce</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intermediate data in case of PMR is 18468MB for 20GB whichis 92%</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR on Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>total</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hadoop MR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for total</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr ofr pmr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for hmr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hadoop</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>India,8workers,1woker/node, 128MB chunk, 8 reduces,varying input data size(GB)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>default replication factor - 2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>scp</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>paramiko</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>File in GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCP</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Paramiko</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>t-scp% of t-paramiko</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data size in GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>effective data transfer in GB in HMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>effective data transfer in GB in PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>%improvement of PMR(paramiko) over HMR(SCP)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>%improvement of PMR(SCP) over HMR(SCP)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 to B</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 to LOCAL</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 to A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>negligible file transfer time</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>effective data transfer involved in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total intermediate data produced in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-0</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>of weissmann paper..</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>related work</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>running bulk of applications on setup of machines.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>16GB wordcount , local mr, 8 workers, 128MB chunk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transferred between map and reduce phase</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machines used India, hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chunk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffletime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce phase</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intermediatedata</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduces</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-2</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-3</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-4</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-5r</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>rreduce-6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-7</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of concurent transfers</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>effective data transfer</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 5952 MB from India-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (5952*2) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chunk</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffletime</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce phase</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (5932*2) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 5932 MB from India-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>40GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>40GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>29minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> in 29 minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>29mins</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local Data in MB transferred within India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>time taken to distribute data to remote machines</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>14mins</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;1min</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Remote Data in MB transferred to </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> effective data transfer in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>remote data distribution= 7mins</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR on India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR on Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 3120MB from India-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>total intermediate data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>30GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>60GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>60GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 5932 MB from hotel-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (5932*3) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce-6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>average</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>120GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>30GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 8946 MB from hotel-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (8946*3) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Distributed-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>120GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of concurrent pilot transfers are 8*(2-1)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB divided into 10GB on india, 10GB hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hadoop MR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>average</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>40GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>80GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>DMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer 8946 MB from India-&gt;hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Combine LMR on (8946*2) MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>80GB(replicated)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqeuences</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>20GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>14minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> in 14 minutes</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remote Data in MB transferred to India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machines</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>India</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hotel</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intermdiate data generated in MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to transfer local data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;1sec</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average reduce data</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Total data exchanged is </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. if its reduce intensive , then it takes more time.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. it is forced to move the data to location where data transfer is high..</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. With efficient file transfer protocols, pilot-DMR proves to be better.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>10GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local PMR on 6240MB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Transfer 3120MB using SCP</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>9GB</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.5 LOCAL</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -924,11 +940,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1025,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1069,6 +1086,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,11 +1339,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="525300904"/>
-        <c:axId val="525286808"/>
+        <c:axId val="525432824"/>
+        <c:axId val="528915960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="525300904"/>
+        <c:axId val="525432824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,14 +1367,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="525286808"/>
+        <c:crossAx val="528915960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="525286808"/>
+        <c:axId val="528915960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,7 +1398,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="525300904"/>
+        <c:crossAx val="525432824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1742,31 +1760,31 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="523400344"/>
-        <c:axId val="523397192"/>
+        <c:axId val="526093416"/>
+        <c:axId val="562607560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523400344"/>
+        <c:axId val="526093416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523397192"/>
+        <c:crossAx val="562607560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523397192"/>
+        <c:axId val="562607560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523400344"/>
+        <c:crossAx val="526093416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2314,11 +2332,11 @@
         </c:ser>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="525241672"/>
-        <c:axId val="525237704"/>
+        <c:axId val="463151448"/>
+        <c:axId val="463223544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="525241672"/>
+        <c:axId val="463151448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,14 +2371,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525237704"/>
+        <c:crossAx val="463223544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="525237704"/>
+        <c:axId val="463223544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3000.0"/>
@@ -2397,7 +2415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525241672"/>
+        <c:crossAx val="463151448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500.0"/>
@@ -2660,13 +2678,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2279.393333333333</c:v>
+                  <c:v>2279.39333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4239.813333333334</c:v>
+                  <c:v>4239.81333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7884.053333333333</c:v>
+                  <c:v>7884.05333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7884.053333333333</c:v>
@@ -2675,11 +2693,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="523325416"/>
-        <c:axId val="523314056"/>
+        <c:axId val="459555688"/>
+        <c:axId val="459622424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523325416"/>
+        <c:axId val="459555688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,14 +2721,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523314056"/>
+        <c:crossAx val="459622424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523314056"/>
+        <c:axId val="459622424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +2753,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523325416"/>
+        <c:crossAx val="459555688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2786,6 +2804,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2832,23 +2851,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="524419464"/>
-        <c:axId val="524416440"/>
+        <c:axId val="490532296"/>
+        <c:axId val="562282584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="524419464"/>
+        <c:axId val="490532296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524416440"/>
+        <c:crossAx val="562282584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="524416440"/>
+        <c:axId val="562282584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,13 +2875,14 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524419464"/>
+        <c:crossAx val="490532296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2897,6 +2917,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2943,23 +2964,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="524373688"/>
-        <c:axId val="524370712"/>
+        <c:axId val="489828520"/>
+        <c:axId val="490080504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="524373688"/>
+        <c:axId val="489828520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524370712"/>
+        <c:crossAx val="490080504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="524370712"/>
+        <c:axId val="490080504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2967,13 +2988,14 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="524373688"/>
+        <c:crossAx val="489828520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3167,38 +3189,37 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="457372408"/>
-        <c:axId val="457375464"/>
+        <c:axId val="528929128"/>
+        <c:axId val="526222984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457372408"/>
+        <c:axId val="528929128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457375464"/>
+        <c:crossAx val="526222984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457375464"/>
+        <c:axId val="526222984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457372408"/>
+        <c:crossAx val="528929128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3912,7 +3933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K33" sqref="K33:N33"/>
     </sheetView>
   </sheetViews>
@@ -3920,7 +3941,7 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="B2" s="9" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -3930,45 +3951,45 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="26">
       <c r="A13" s="3" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>216</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>217</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4091,28 +4112,28 @@
         <v>69.652011250000001</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -4139,7 +4160,7 @@
     </row>
     <row r="22" spans="1:18" s="7" customFormat="1">
       <c r="A22" s="6" t="s">
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="J22"/>
       <c r="K22" s="11"/>
@@ -4172,28 +4193,28 @@
     </row>
     <row r="24" spans="1:18" s="2" customFormat="1" ht="78">
       <c r="A24" s="4" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>216</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>52</v>
+        <v>217</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="J24">
         <v>2</v>
@@ -4429,7 +4450,7 @@
     </row>
     <row r="33" spans="1:18">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>223</v>
       </c>
       <c r="J33">
         <v>16</v>
@@ -4474,7 +4495,7 @@
     </row>
     <row r="43" spans="1:18">
       <c r="J43" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -4512,24 +4533,24 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="3" t="s">
-        <v>51</v>
+        <v>216</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>52</v>
+        <v>217</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="3" t="s">
-        <v>180</v>
+        <v>92</v>
       </c>
       <c r="B46">
         <v>164.37300000000002</v>
@@ -4547,7 +4568,7 @@
         <v>2929.2380000000003</v>
       </c>
       <c r="H46" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="I46" s="5">
         <v>684.23799999999994</v>
@@ -4567,7 +4588,7 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="3" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
       <c r="B47" s="1">
         <v>138.96699999999998</v>
@@ -4585,7 +4606,7 @@
         <v>2437.4606666666668</v>
       </c>
       <c r="H47" t="s">
-        <v>57</v>
+        <v>222</v>
       </c>
       <c r="I47" s="5">
         <v>473.4563333333333</v>
@@ -4605,7 +4626,7 @@
     </row>
     <row r="48" spans="1:18">
       <c r="H48" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="I48">
         <v>33.993099001840605</v>
@@ -4625,7 +4646,7 @@
     </row>
     <row r="49" spans="8:13">
       <c r="H49" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="I49">
         <v>127.57381609687643</v>
@@ -4687,10 +4708,8 @@
       <c r="G81" s="5"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4702,10 +4721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:V172"/>
+  <dimension ref="A1:Z172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4713,49 +4732,80 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>214</v>
       </c>
       <c r="B2">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
+        <v>213</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4">
+        <v>136</v>
+      </c>
+      <c r="J4">
+        <f>3120/1024</f>
+        <v>3.046875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5">
+        <v>197</v>
+      </c>
+      <c r="J5">
+        <f>J4/8</f>
+        <v>0.380859375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
+        <v>91</v>
+      </c>
+      <c r="H6">
+        <f>(5932*2)/1024</f>
+        <v>11.5859375</v>
+      </c>
+      <c r="J6">
+        <f>1248/1024</f>
+        <v>1.21875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21" t="s">
-        <v>36</v>
+        <v>201</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -4765,175 +4815,219 @@
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
     </row>
-    <row r="8" spans="1:22" s="10" customFormat="1" ht="65">
+    <row r="8" spans="1:26" s="10" customFormat="1" ht="65">
       <c r="A8" s="19" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>41</v>
+        <v>206</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="G8" s="19"/>
       <c r="I8" s="19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="11">
         <v>1996.0322450000001</v>
       </c>
       <c r="B9" s="11">
         <v>1742.8240000000001</v>
       </c>
-      <c r="C9" s="11">
-        <f>3120/43.5</f>
-        <v>71.724137931034477</v>
+      <c r="C9">
+        <v>88.90019531249996</v>
       </c>
       <c r="D9" s="11">
-        <v>637.42506249999997</v>
+        <v>197.4250625</v>
       </c>
       <c r="E9" s="11">
         <f>MAX(A9:B9)+C9+D9</f>
-        <v>2705.1814454310347</v>
+        <v>2282.3575028125001</v>
       </c>
       <c r="F9" s="17">
         <v>3120</v>
       </c>
       <c r="K9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
+        <v>20</v>
+      </c>
+      <c r="X9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="11">
         <v>1960.294715</v>
       </c>
       <c r="B10" s="11">
         <v>1813.597</v>
       </c>
-      <c r="C10" s="11">
-        <f>3120/43.5</f>
-        <v>71.724137931034477</v>
+      <c r="C10">
+        <v>88.90019531249996</v>
       </c>
       <c r="D10" s="11">
-        <v>649.32174218750004</v>
+        <v>199.32174218750001</v>
       </c>
       <c r="E10" s="11">
         <f>MAX(A10:B10)+C10+D10</f>
-        <v>2681.3405951185346</v>
+        <v>2248.5166525</v>
       </c>
       <c r="F10" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G10">
         <f>AVERAGE(E9:E11)</f>
-        <v>2652.2825510560347</v>
+        <v>2232.7919417708331</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>224</v>
       </c>
       <c r="I10">
         <v>19029605</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="Z10">
+        <f>(19100/2)/8</f>
+        <v>1193.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="11">
         <v>1875.3710450000001</v>
       </c>
       <c r="B11" s="11">
         <v>1738.2349999999999</v>
       </c>
-      <c r="C11" s="11">
-        <f>3120/43.5</f>
-        <v>71.724137931034477</v>
+      <c r="C11">
+        <v>88.90019531249996</v>
       </c>
       <c r="D11" s="11">
-        <v>623.23042968749996</v>
+        <v>203.23042968749999</v>
       </c>
       <c r="E11" s="11">
         <f>MAX(A11:B11)+C11+D11</f>
-        <v>2570.3256126185343</v>
+        <v>2167.5016700000001</v>
       </c>
       <c r="F11" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G11">
         <f>1.96*(STDEV(E9:E11)/SQRT(3))</f>
-        <v>81.442668757892889</v>
+        <v>66.787945274149649</v>
       </c>
       <c r="K11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
+        <v>21</v>
+      </c>
+      <c r="W11" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11">
+        <v>233.42</v>
+      </c>
+      <c r="Z11">
+        <f>1193.75/1024</f>
+        <v>1.165771484375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="K12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
+        <v>22</v>
+      </c>
+      <c r="W12">
+        <f>3120/1024</f>
+        <v>3.046875</v>
+      </c>
+      <c r="X12">
+        <f>W12*X11</f>
+        <v>711.20156249999991</v>
+      </c>
+      <c r="Z12">
+        <f>Z11*233.42</f>
+        <v>272.1143798828125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="W13">
+        <f>W12/8</f>
+        <v>0.380859375</v>
+      </c>
+      <c r="X13">
+        <f>W13*233.42</f>
+        <v>88.900195312499989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="E14" t="s">
-        <v>61</v>
+        <v>226</v>
       </c>
       <c r="H14">
         <f>(F9-F17)/F17*100</f>
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:26">
       <c r="I15">
         <f>(G10-G18)/G18*100</f>
-        <v>10.423280970223924</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="65">
+        <v>-3.9903017397377276</v>
+      </c>
+      <c r="W15">
+        <f>((5932)/8)/1024</f>
+        <v>0.72412109375</v>
+      </c>
+      <c r="X15">
+        <f>W15*233.42</f>
+        <v>169.02434570312499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="65">
       <c r="A16" s="22" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -4944,15 +5038,15 @@
         <v>1542.21</v>
       </c>
       <c r="C17">
-        <f>7*60</f>
-        <v>420</v>
+        <f>350</f>
+        <v>350</v>
       </c>
       <c r="D17">
         <v>242.78</v>
       </c>
       <c r="E17">
         <f>SUM(A17:D17)</f>
-        <v>2468.3000000000002</v>
+        <v>2398.3000000000002</v>
       </c>
       <c r="F17" s="17">
         <v>1248</v>
@@ -4961,7 +5055,7 @@
         <v>19100</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="J17">
         <f>SUM(A17,B17,D17)+(1248/8.7)</f>
@@ -4983,7 +5077,7 @@
       </c>
       <c r="V17">
         <f>(G10-J20)/J20*100</f>
-        <v>24.928626168035727</v>
+        <v>5.1696508327999231</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -4994,21 +5088,21 @@
         <v>1441.11</v>
       </c>
       <c r="C18">
-        <v>423</v>
+        <v>345</v>
       </c>
       <c r="D18">
         <v>239.64</v>
       </c>
       <c r="E18">
         <f>SUM(A18:D18)</f>
-        <v>2358.3399999999997</v>
+        <v>2280.3399999999997</v>
       </c>
       <c r="F18" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G18">
         <f>AVERAGE(E17:E19)</f>
-        <v>2401.9233333333332</v>
+        <v>2325.5899999999997</v>
       </c>
       <c r="J18">
         <f t="shared" ref="J18:J19" si="0">SUM(A18,B18,D18)+(1248/8.7)</f>
@@ -5036,7 +5130,7 @@
       </c>
       <c r="V18">
         <f>((G30-L45)/L45)*100</f>
-        <v>30.018305344977225</v>
+        <v>6.4748832027290568</v>
       </c>
     </row>
     <row r="19" spans="1:22">
@@ -5047,21 +5141,21 @@
         <v>1446.79</v>
       </c>
       <c r="C19">
-        <v>424</v>
+        <v>343</v>
       </c>
       <c r="D19">
         <v>240.34</v>
       </c>
       <c r="E19">
         <f>SUM(A19:D19)</f>
-        <v>2379.13</v>
+        <v>2298.13</v>
       </c>
       <c r="F19" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G19">
         <f>1.96*(STDEV(E17:E19)/SQRT(3))</f>
-        <v>66.104153343773305</v>
+        <v>71.963227717505674</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
@@ -5090,12 +5184,12 @@
       </c>
       <c r="V19">
         <f>((G56-L63)/L63)*100</f>
-        <v>25.694223221716751</v>
+        <v>6.2088587461652311</v>
       </c>
     </row>
     <row r="20" spans="1:22">
       <c r="I20" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="J20">
         <f>AVERAGE(J17:J19)</f>
@@ -5112,11 +5206,55 @@
     </row>
     <row r="21" spans="1:22">
       <c r="I21" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="J21">
         <f>1.96*(STDEV(J17:J19)/SQRT(3))</f>
         <v>68.260444569707076</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="D22">
+        <f>(19100/2)/1024</f>
+        <v>9.326171875</v>
+      </c>
+      <c r="G22">
+        <f>19100/1024</f>
+        <v>18.65234375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="39">
+      <c r="T23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="T24">
+        <v>20</v>
+      </c>
+      <c r="U24" s="27">
+        <f>MAX(A9:B9)+88.9+D9</f>
+        <v>2282.3573074999999</v>
+      </c>
+      <c r="V24">
+        <f>SUM(A17:D17)</f>
+        <v>2398.3000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="T25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="T26">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:22">
@@ -5125,7 +5263,7 @@
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -5137,22 +5275,22 @@
     </row>
     <row r="28" spans="1:22" ht="65">
       <c r="A28" s="19" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:22">
@@ -5164,18 +5302,22 @@
         <v>2914.9259999999999</v>
       </c>
       <c r="C29" s="11">
-        <f>5932/43.5</f>
-        <v>136.36781609195401</v>
+        <f>169.34</f>
+        <v>169.34</v>
       </c>
       <c r="D29">
-        <v>1254.23</v>
+        <v>354.23</v>
       </c>
       <c r="E29" s="11">
         <f>MAX(A29:B29)+C29+D29</f>
-        <v>4819.4278160919539</v>
+        <v>3952.4</v>
       </c>
       <c r="F29" s="17">
         <v>5932</v>
+      </c>
+      <c r="H29">
+        <f>5932/1024</f>
+        <v>5.79296875</v>
       </c>
     </row>
     <row r="30" spans="1:22">
@@ -5186,35 +5328,43 @@
       <c r="B30">
         <v>2837.6559999999999</v>
       </c>
-      <c r="C30" s="11">
-        <f t="shared" ref="C30:C31" si="1">5932/43.5</f>
-        <v>136.36781609195401</v>
+      <c r="C30" s="25">
+        <f t="shared" ref="C30:C31" si="1">169.34</f>
+        <v>169.34</v>
       </c>
       <c r="D30">
-        <v>1263.3399999999999</v>
+        <v>363.34</v>
       </c>
       <c r="E30" s="11">
         <f>MAX(A30:B30)+C30+D30</f>
-        <v>4832.7978160919538</v>
+        <v>3965.77</v>
       </c>
       <c r="F30" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G30">
         <f>AVERAGE(E29:E31)</f>
-        <v>4788.1521494252875</v>
+        <v>3921.1243333333332</v>
+      </c>
+      <c r="H30">
+        <f>H29/8</f>
+        <v>0.72412109375</v>
+      </c>
+      <c r="I30">
+        <f>F41/1024</f>
+        <v>2.4287109375</v>
       </c>
       <c r="Q30" t="s">
-        <v>187</v>
+        <v>99</v>
       </c>
       <c r="R30" t="s">
-        <v>188</v>
+        <v>100</v>
       </c>
       <c r="S30" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="T30" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:22" s="2" customFormat="1">
@@ -5225,32 +5375,32 @@
       <c r="B31">
         <v>2869.0210000000002</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="25">
         <f t="shared" si="1"/>
-        <v>136.36781609195401</v>
+        <v>169.34</v>
       </c>
       <c r="D31" s="2">
-        <v>1247.3430000000001</v>
+        <v>347.34300000000002</v>
       </c>
       <c r="E31" s="11">
         <f>MAX(A31:B31)+C31+D31</f>
-        <v>4712.2308160919538</v>
+        <v>3845.203</v>
       </c>
       <c r="F31" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G31">
         <f>1.96*(STDEV(E29:E31)/SQRT(3))</f>
         <v>74.786486497903951</v>
       </c>
       <c r="P31" t="s">
-        <v>184</v>
+        <v>96</v>
       </c>
       <c r="Q31">
         <v>2652.2825510560347</v>
       </c>
       <c r="R31">
-        <v>2279.3933333333334</v>
+        <v>2279.3933333333298</v>
       </c>
       <c r="S31">
         <v>81.442668757892889</v>
@@ -5260,7 +5410,7 @@
       </c>
       <c r="U31">
         <f>(Q31-R31)/R31*100</f>
-        <v>16.359143122411279</v>
+        <v>16.359143122411464</v>
       </c>
     </row>
     <row r="32" spans="1:22">
@@ -5270,16 +5420,16 @@
         <v>138.52030558906313</v>
       </c>
       <c r="M32" t="s">
-        <v>19</v>
+        <v>184</v>
       </c>
       <c r="P32" t="s">
-        <v>185</v>
+        <v>97</v>
       </c>
       <c r="Q32">
         <v>4528.8221494252866</v>
       </c>
       <c r="R32">
-        <v>4239.8133333333335</v>
+        <v>4239.8133333333299</v>
       </c>
       <c r="S32">
         <v>74.786486497903951</v>
@@ -5289,21 +5439,21 @@
       </c>
       <c r="U32">
         <f t="shared" ref="U32:U34" si="2">(Q32-R32)/R32*100</f>
-        <v>6.8165457620450214</v>
+        <v>6.8165457620451138</v>
       </c>
     </row>
     <row r="33" spans="1:21">
       <c r="M33" t="s">
-        <v>20</v>
+        <v>185</v>
       </c>
       <c r="P33" t="s">
-        <v>186</v>
+        <v>98</v>
       </c>
       <c r="Q33">
         <v>8375.575505747127</v>
       </c>
       <c r="R33">
-        <v>7884.0533333333333</v>
+        <v>7884.0533333333296</v>
       </c>
       <c r="S33">
         <v>32.578079537658802</v>
@@ -5313,15 +5463,15 @@
       </c>
       <c r="U33">
         <f t="shared" si="2"/>
-        <v>6.2343841629744645</v>
+        <v>6.2343841629745125</v>
       </c>
     </row>
     <row r="34" spans="1:21">
       <c r="M34" t="s">
-        <v>21</v>
+        <v>186</v>
       </c>
       <c r="P34" t="s">
-        <v>191</v>
+        <v>1</v>
       </c>
       <c r="Q34">
         <v>7606.7479195402293</v>
@@ -5342,36 +5492,36 @@
     </row>
     <row r="36" spans="1:21">
       <c r="B36" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:21">
       <c r="H37">
         <f>(G30-G42)/G42*100</f>
-        <v>12.933088628712127</v>
+        <v>-4.4128683843581085</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="65">
       <c r="A40" s="16" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -5383,15 +5533,14 @@
         <v>2759.67</v>
       </c>
       <c r="C41">
-        <f>14*60+3</f>
-        <v>843</v>
+        <v>704</v>
       </c>
       <c r="D41">
         <v>415.92</v>
       </c>
       <c r="E41">
         <f>SUM(A41:D41)</f>
-        <v>4271.83</v>
+        <v>4132.83</v>
       </c>
       <c r="F41" s="17">
         <v>2487</v>
@@ -5413,7 +5562,7 @@
         <v>0.11484290357529794</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>0</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -5424,25 +5573,24 @@
         <v>2768.13</v>
       </c>
       <c r="C42">
-        <f>14*60</f>
-        <v>840</v>
+        <v>702</v>
       </c>
       <c r="D42">
         <v>404.53</v>
       </c>
       <c r="E42">
         <f t="shared" ref="E42:E43" si="3">SUM(A42:D42)</f>
-        <v>4273.09</v>
+        <v>4135.09</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G42">
         <f>AVERAGE(E41:E43)</f>
-        <v>4239.8133333333335</v>
+        <v>4102.1466666666665</v>
       </c>
       <c r="I42" s="20" t="s">
-        <v>193</v>
+        <v>3</v>
       </c>
       <c r="L42">
         <f>SUM(B42,D42,A42)+(F41/8.7)</f>
@@ -5457,21 +5605,21 @@
         <v>2668.96</v>
       </c>
       <c r="C43">
-        <v>846</v>
+        <v>710</v>
       </c>
       <c r="D43">
         <v>395.24</v>
       </c>
       <c r="E43">
         <f t="shared" si="3"/>
-        <v>4174.5200000000004</v>
+        <v>4038.5200000000004</v>
       </c>
       <c r="F43" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G43">
         <f>1.96*(STDEV(E41:E43)/SQRT(3))</f>
-        <v>63.991437974886438</v>
+        <v>62.367243459734112</v>
       </c>
       <c r="I43">
         <f>19029605*2</f>
@@ -5490,10 +5638,10 @@
     </row>
     <row r="45" spans="1:21">
       <c r="H45" t="s">
-        <v>178</v>
+        <v>90</v>
       </c>
       <c r="K45" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="L45">
         <f>AVERAGE(L42:L44)</f>
@@ -5502,16 +5650,16 @@
     </row>
     <row r="46" spans="1:21">
       <c r="C46" t="s">
-        <v>62</v>
+        <v>227</v>
       </c>
       <c r="D46" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="F46" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="K46" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="L46">
         <f>1.96*(STDEV(L42:L44)/SQRT(3))</f>
@@ -5520,7 +5668,7 @@
     </row>
     <row r="52" spans="1:12" s="21" customFormat="1">
       <c r="E52" s="21" t="s">
-        <v>37</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -5528,22 +5676,22 @@
     </row>
     <row r="54" spans="1:12" ht="65">
       <c r="A54" s="19" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>190</v>
+        <v>0</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -5559,14 +5707,26 @@
         <v>205.65517241379311</v>
       </c>
       <c r="D55">
-        <v>1978.21</v>
+        <v>678.21</v>
       </c>
       <c r="E55" s="11">
         <f>MAX(A55:B55)+C55+D55</f>
-        <v>8392.4551724137928</v>
+        <v>7092.4551724137937</v>
       </c>
       <c r="F55" s="20">
         <v>8946</v>
+      </c>
+      <c r="H55">
+        <f>8946/1024</f>
+        <v>8.736328125</v>
+      </c>
+      <c r="I55">
+        <f>36454.269/1024</f>
+        <v>35.5998720703125</v>
+      </c>
+      <c r="K55">
+        <f>(8946*2)/1024</f>
+        <v>17.47265625</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -5581,18 +5741,26 @@
         <v>205.65517241379311</v>
       </c>
       <c r="D56">
-        <v>1970.36</v>
+        <v>670.36</v>
       </c>
       <c r="E56" s="11">
         <f t="shared" ref="E56:E57" si="5">MAX(A56:B56)+C56+D56</f>
-        <v>8410.8611724137936</v>
+        <v>7110.8611724137927</v>
       </c>
       <c r="F56" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G56">
         <f>AVERAGE(E55:E57)</f>
-        <v>8385.9088390804609</v>
+        <v>7085.90883908046</v>
+      </c>
+      <c r="H56">
+        <f>H55/8</f>
+        <v>1.092041015625</v>
+      </c>
+      <c r="I56">
+        <f>I55/8</f>
+        <v>4.4499840087890625</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -5607,44 +5775,44 @@
         <v>205.65517241379311</v>
       </c>
       <c r="D57" s="2">
-        <v>1985.31</v>
+        <v>685.31</v>
       </c>
       <c r="E57" s="11">
         <f t="shared" si="5"/>
-        <v>8354.4101724137927</v>
+        <v>7054.4101724137927</v>
       </c>
       <c r="F57" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G57">
         <f>1.96*(STDEV(E55:E57)/SQRT(3))</f>
-        <v>32.578079537658802</v>
+        <v>32.578079538537381</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="65">
       <c r="A59" s="16" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>193</v>
+        <v>3</v>
       </c>
       <c r="L59" s="22" t="s">
-        <v>0</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -5656,15 +5824,15 @@
         <v>4859.67</v>
       </c>
       <c r="C60">
-        <f>29*60+3</f>
-        <v>1743</v>
+        <f>1456</f>
+        <v>1456</v>
       </c>
       <c r="D60">
         <v>795.92</v>
       </c>
       <c r="E60">
         <f>SUM(A60:D60)</f>
-        <v>7951.59</v>
+        <v>7664.59</v>
       </c>
       <c r="F60" s="17">
         <v>4425</v>
@@ -5691,22 +5859,21 @@
         <v>4790.34</v>
       </c>
       <c r="C61">
-        <f>28*60</f>
-        <v>1680</v>
+        <v>1432</v>
       </c>
       <c r="D61">
         <v>764.53</v>
       </c>
       <c r="E61">
         <f t="shared" ref="E61:E62" si="6">SUM(A61:D61)</f>
-        <v>7794.87</v>
+        <v>7546.87</v>
       </c>
       <c r="F61" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G61">
         <f>AVERAGE(E60:E62)</f>
-        <v>7884.0533333333333</v>
+        <v>7607.0533333333333</v>
       </c>
       <c r="L61">
         <f>SUM(B61,D61,A61)+(4425/8.7)</f>
@@ -5722,22 +5889,21 @@
         <v>4798.96</v>
       </c>
       <c r="C62">
-        <f>29*60</f>
-        <v>1740</v>
+        <v>1444</v>
       </c>
       <c r="D62">
         <v>815.24</v>
       </c>
       <c r="E62">
         <f t="shared" si="6"/>
-        <v>7905.7</v>
+        <v>7609.7</v>
       </c>
       <c r="F62" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G62">
         <f>1.96*(STDEV(E60:E62)/SQRT(3))</f>
-        <v>91.174930715904665</v>
+        <v>66.656842662386921</v>
       </c>
       <c r="L62">
         <f>SUM(B62,D62,A62)+(4425/8.7)</f>
@@ -5750,7 +5916,7 @@
         <v>102.16949152542374</v>
       </c>
       <c r="K63" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="L63">
         <f>AVERAGE(L60:L62)</f>
@@ -5759,7 +5925,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="K64" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="L64">
         <f>1.96*(STDEV(L60:L62)/SQRT(3))</f>
@@ -5768,32 +5934,32 @@
     </row>
     <row r="65" spans="1:10">
       <c r="B65" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="21" customFormat="1">
       <c r="E66" s="21" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="65">
       <c r="A70" s="19" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -5842,7 +6008,7 @@
         <v>7622.033586206896</v>
       </c>
       <c r="F72" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G72">
         <f>AVERAGE(E71:E73)</f>
@@ -5875,7 +6041,7 @@
         <v>7585.5825862068959</v>
       </c>
       <c r="F73" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G73">
         <f>1.96*(STDEV(E71:E73)/SQRT(3))</f>
@@ -5885,7 +6051,7 @@
     <row r="78" spans="1:10">
       <c r="G78">
         <f>AVERAGE(D55:D57)</f>
-        <v>1977.9599999999998</v>
+        <v>677.96</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -5893,13 +6059,13 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="E91" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -5917,26 +6083,26 @@
         <v>5.4</v>
       </c>
       <c r="C122" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="2:15">
       <c r="C148" t="s">
-        <v>2</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="2:15" ht="26">
       <c r="B149" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="C149" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D149" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
     </row>
     <row r="150" spans="2:15">
@@ -6019,30 +6185,30 @@
     </row>
     <row r="157" spans="2:15">
       <c r="C157" t="s">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="I157" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="J157" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="K157" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
     </row>
     <row r="158" spans="2:15" ht="26">
       <c r="B158" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="C158" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D158" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="I158">
         <v>1</v>
@@ -6304,122 +6470,122 @@
   <sheetData>
     <row r="1" spans="2:8">
       <c r="C1" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>214</v>
+        <v>24</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>216</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:8">
       <c r="B2" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" t="s">
-        <v>217</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:8">
       <c r="C3" t="s">
-        <v>222</v>
+        <v>32</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>215</v>
+        <v>25</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>55</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="2:8">
       <c r="G7" t="s">
-        <v>220</v>
+        <v>30</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="C8" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="F8" t="s">
-        <v>219</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:8">
       <c r="B9" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:8">
       <c r="C10" t="s">
-        <v>223</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>183</v>
       </c>
       <c r="F10" t="s">
-        <v>219</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="2:8">
       <c r="G11" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="39">
       <c r="A20" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="2" customFormat="1">
       <c r="A21" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>9862</v>
@@ -6436,7 +6602,7 @@
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
       <c r="J21"/>
       <c r="K21"/>
@@ -6485,10 +6651,10 @@
         <v>9267</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>179</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -6504,7 +6670,7 @@
     </row>
     <row r="28" spans="1:13">
       <c r="B28" t="s">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <v>9838</v>
@@ -6547,58 +6713,58 @@
     </row>
     <row r="32" spans="1:13">
       <c r="D32" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="C34" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="E34" t="s">
-        <v>153</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="52">
       <c r="A40" s="2" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>205</v>
+        <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>208</v>
+        <v>18</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>209</v>
+        <v>19</v>
       </c>
       <c r="K40" s="16" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>202</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="C41">
         <v>9862</v>
@@ -6612,7 +6778,7 @@
         <v>4604</v>
       </c>
       <c r="F41" t="s">
-        <v>207</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>7</v>
@@ -6626,7 +6792,7 @@
         <v>9267</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="K41" s="17">
         <f>MAX('10GB'!E21:E24,'10GB'!E27:E30)</f>
@@ -6635,10 +6801,10 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>204</v>
+        <v>14</v>
       </c>
       <c r="C42">
         <v>9838</v>
@@ -6652,7 +6818,7 @@
         <v>4663</v>
       </c>
       <c r="F42" t="s">
-        <v>207</v>
+        <v>17</v>
       </c>
       <c r="G42">
         <v>7</v>
@@ -6665,7 +6831,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="J43" s="18" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
       <c r="K43" s="17">
         <f>3120</f>
@@ -6673,6 +6839,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -6695,39 +6862,39 @@
   <sheetData>
     <row r="1" spans="1:12" ht="65">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>205</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>143</v>
+        <v>55</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>209</v>
+        <v>19</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>18468</v>
@@ -6741,17 +6908,17 @@
         <v>9184</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="H2">
         <f>SUM(D2:D3)</f>
         <v>18456</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="K2" s="17">
         <f>MAX(E11:E14,E17:E20)</f>
@@ -6764,10 +6931,10 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>18468</v>
@@ -6781,10 +6948,10 @@
         <v>9296</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="H3">
         <f>SUM(D2:D3)</f>
@@ -6794,7 +6961,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="J4" s="18" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
       <c r="K4" s="17">
         <f>2980+2985</f>
@@ -6803,27 +6970,27 @@
     </row>
     <row r="10" spans="1:12" ht="52">
       <c r="A10" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>18468</v>
@@ -6871,18 +7038,18 @@
         <v>4552</v>
       </c>
       <c r="I14" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="D16" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>198</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -6898,7 +7065,7 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>18468</v>
@@ -6936,6 +7103,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -6948,49 +7116,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I12" sqref="I12:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:11" ht="65">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>205</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>143</v>
+        <v>55</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>209</v>
+        <v>19</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>147</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>36454.269</v>
@@ -7004,17 +7172,17 @@
         <v>17233</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="H2">
         <f>SUM(D2:D3)</f>
         <v>34978</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>149</v>
+        <v>61</v>
       </c>
       <c r="K2" s="17">
         <f>MAX(E11:E14,E17:E20)</f>
@@ -7023,10 +7191,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>36454.269</v>
@@ -7040,10 +7208,10 @@
         <v>17123</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>53</v>
       </c>
       <c r="H3">
         <f>SUM(D2:D3)</f>
@@ -7053,7 +7221,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="J4" s="18" t="s">
-        <v>148</v>
+        <v>60</v>
       </c>
       <c r="K4" s="17">
         <f>5952</f>
@@ -7062,27 +7230,27 @@
     </row>
     <row r="10" spans="1:11" ht="52">
       <c r="A10" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>142</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>36454.269</v>
@@ -7116,7 +7284,7 @@
         <v>12.138496042809143</v>
       </c>
       <c r="I12" t="s">
-        <v>25</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -7151,13 +7319,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="D16" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -7177,10 +7345,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>36454.269</v>
@@ -7235,9 +7403,17 @@
         <v>0.91349999999999998</v>
       </c>
     </row>
+    <row r="30" spans="1:8">
+      <c r="C30">
+        <f>(C11+C18)/1024</f>
+        <v>71.199744140625</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7265,7 +7441,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -7277,25 +7453,25 @@
     </row>
     <row r="2" spans="1:16" ht="65">
       <c r="A2" s="19" t="s">
-        <v>154</v>
+        <v>66</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>42</v>
+        <v>207</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>40</v>
+        <v>205</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="H2" s="19"/>
       <c r="O2">
@@ -7359,7 +7535,7 @@
         <v>3014.5888529310346</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="H4">
         <f>AVERAGE(F3:F5)</f>
@@ -7395,7 +7571,7 @@
         <v>2882.3651829310347</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="H5">
         <f>1.96*(STDEV(F3:F5)/SQRT(3))</f>
@@ -7447,25 +7623,25 @@
     </row>
     <row r="11" spans="1:16" ht="65">
       <c r="A11" s="22" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -7494,13 +7670,13 @@
         <v>28396</v>
       </c>
       <c r="L12" t="s">
-        <v>159</v>
+        <v>71</v>
       </c>
       <c r="M12" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="N12" t="s">
-        <v>175</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -7522,14 +7698,14 @@
         <v>2263.6266666666666</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="G13">
         <f>AVERAGE(E12:E14)</f>
         <v>2318.4266666666667</v>
       </c>
       <c r="K13" t="s">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="L13">
         <v>2984.3501395977014</v>
@@ -7560,14 +7736,14 @@
         <v>2328.2266666666669</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="G14">
         <f>1.96*(STDEV(E12:E14)/SQRT(3))</f>
         <v>57.278072779497222</v>
       </c>
       <c r="K14" t="s">
-        <v>174</v>
+        <v>86</v>
       </c>
       <c r="L14">
         <v>2416.8599999999997</v>
@@ -7578,7 +7754,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="K17" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
       <c r="L17">
         <v>102.66744486459044</v>
@@ -7592,7 +7768,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="K18" t="s">
-        <v>177</v>
+        <v>89</v>
       </c>
       <c r="L18">
         <v>53.54597837390223</v>
@@ -7607,7 +7783,7 @@
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21" t="s">
-        <v>161</v>
+        <v>73</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
@@ -7619,25 +7795,25 @@
     </row>
     <row r="22" spans="1:14" ht="65">
       <c r="A22" s="19" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>163</v>
+        <v>75</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -7689,7 +7865,7 @@
         <v>5709.8978160919542</v>
       </c>
       <c r="G24" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="H24">
         <f>AVERAGE(F23:F25)</f>
@@ -7719,7 +7895,7 @@
         <v>5851.6078160919533</v>
       </c>
       <c r="G25" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="H25">
         <f>1.96*(STDEV(F23:F25)/SQRT(3))</f>
@@ -7735,25 +7911,25 @@
     </row>
     <row r="29" spans="1:14" ht="65">
       <c r="A29" s="22" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -7801,7 +7977,7 @@
         <v>4508.99</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
       <c r="G31">
         <f>AVERAGE(E30:E32)</f>
@@ -7826,7 +8002,7 @@
         <v>4642.45</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="G32">
         <f>1.96*(STDEV(E30:E32)/SQRT(3))</f>
@@ -7848,7 +8024,7 @@
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
       <c r="E36" s="21" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
@@ -7860,25 +8036,25 @@
     </row>
     <row r="37" spans="1:12" ht="65">
       <c r="A37" s="19" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>189</v>
+        <v>101</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>172</v>
+        <v>84</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -7929,7 +8105,7 @@
         <v>9408.8711724137938</v>
       </c>
       <c r="G39" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="H39">
         <f>AVERAGE(F38:F40)</f>
@@ -7958,7 +8134,7 @@
         <v>9256.9201724137929</v>
       </c>
       <c r="G40" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="H40">
         <f>1.96*(STDEV(F38:F40)/SQRT(3))</f>
@@ -7973,25 +8149,25 @@
     </row>
     <row r="44" spans="1:12" ht="65">
       <c r="A44" s="22" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>45</v>
+        <v>210</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>46</v>
+        <v>211</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -8042,9 +8218,9 @@
       <c r="F47" s="20"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -8077,45 +8253,45 @@
     </row>
     <row r="7" spans="1:12" ht="39">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>9862</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="E8">
         <f>SUM(F8:H8)</f>
@@ -8134,12 +8310,12 @@
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="E9">
         <f>SUM(F9:H9)</f>
@@ -8160,7 +8336,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="D10" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="E10">
         <f>SUM(F10:H10)</f>
@@ -8181,18 +8357,18 @@
     </row>
     <row r="11" spans="1:12">
       <c r="L11" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>9267</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="E12">
         <v>3463</v>
@@ -8216,7 +8392,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="D13" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="E13">
         <v>3568</v>
@@ -8236,7 +8412,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="D14" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="E14">
         <v>3566</v>
@@ -8256,7 +8432,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="K15" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -8267,13 +8443,13 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C17">
         <v>9267</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>78</v>
       </c>
       <c r="E17">
         <v>3531</v>
@@ -8293,7 +8469,7 @@
     </row>
     <row r="18" spans="2:10">
       <c r="D18" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="E18">
         <v>3904</v>
@@ -8335,45 +8511,45 @@
   <sheetData>
     <row r="7" spans="1:12" ht="39">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>18468</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="E8">
         <f>SUM(F8:H8)</f>
@@ -8392,12 +8568,12 @@
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="D9" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="E9">
         <f>SUM(F9:H9)</f>
@@ -8418,7 +8594,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="D10" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="E10">
         <f>SUM(F10:H10)</f>
@@ -8439,18 +8615,18 @@
     </row>
     <row r="11" spans="1:12">
       <c r="L11" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>196</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <v>18468</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="E12">
         <f>SUM(F12:H12)</f>
@@ -8475,7 +8651,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="D13" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="E13">
         <f>SUM(F13:H13)</f>
@@ -8496,7 +8672,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="D14" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="E14">
         <f>SUM(F14:H14)</f>
@@ -8517,7 +8693,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="K15" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -8528,13 +8704,13 @@
     </row>
     <row r="17" spans="2:10">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C17">
         <v>18468</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="E17">
         <f>SUM(F17:H17)</f>
@@ -8555,7 +8731,7 @@
     </row>
     <row r="18" spans="2:10">
       <c r="D18" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="E18">
         <f>SUM(F18:H18)</f>
@@ -8576,7 +8752,7 @@
     </row>
     <row r="25" spans="2:10">
       <c r="H25" t="s">
-        <v>29</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -8603,45 +8779,45 @@
   <sheetData>
     <row r="9" spans="1:12" ht="39">
       <c r="A9" s="2" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>36454.269</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="E10">
         <f>SUM(F10:H10)</f>
@@ -8660,12 +8836,12 @@
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="D11" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="E11">
         <f>SUM(F11:H11)</f>
@@ -8686,7 +8862,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="D12" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="E12">
         <f>SUM(F12:H12)</f>
@@ -8707,18 +8883,18 @@
     </row>
     <row r="13" spans="1:12">
       <c r="L13" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C14">
         <v>36454.269</v>
       </c>
       <c r="D14" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="E14">
         <f>SUM(F14:H14)</f>
@@ -8743,7 +8919,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="D15" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="E15">
         <f>SUM(F15:H15)</f>
@@ -8764,7 +8940,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="D16" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="E16">
         <f>SUM(F16:H16)</f>
@@ -8785,7 +8961,7 @@
     </row>
     <row r="17" spans="2:11">
       <c r="K17" t="s">
-        <v>158</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -8796,13 +8972,13 @@
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="C19">
         <v>36454.269</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="E19">
         <f>SUM(F19:H19)</f>
@@ -8823,7 +8999,7 @@
     </row>
     <row r="20" spans="2:11">
       <c r="D20" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="E20">
         <f>SUM(F20:H20)</f>

</xml_diff>